<commit_message>
Updated experiments file. Added documentation imag, added surface images, added length scale script.
</commit_message>
<xml_diff>
--- a/leki-experiments.xlsx
+++ b/leki-experiments.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lekim\OneDrive\Desktop\School\research-2023\mcgill-natural-faults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A51E88-52B3-4DE0-AFC0-1BF89C4DE83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C1CF0B-5381-4E50-896D-9141F71F345A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JBZQ04 2023-06-16" sheetId="1" r:id="rId1"/>
     <sheet name="AVLY02 2023-07-13" sheetId="2" r:id="rId2"/>
     <sheet name="JBZQ04 2023-7-21" sheetId="3" r:id="rId3"/>
+    <sheet name="smooth 2023-10-26" sheetId="4" r:id="rId4"/>
+    <sheet name="smooth 2023-10-31" sheetId="5" r:id="rId5"/>
+    <sheet name="rough 2023-10-31" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="80">
   <si>
     <t>JBZQ04 against speckled white granite</t>
   </si>
@@ -222,13 +225,68 @@
   <si>
     <t>total distance (mm)</t>
   </si>
+  <si>
+    <t>Apply 7.45 kN for 7.5kN load</t>
+  </si>
+  <si>
+    <t>CYCLE 1</t>
+  </si>
+  <si>
+    <t>CYCLE 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horizontal displacement is about 0.007mm off </t>
+  </si>
+  <si>
+    <t>SHS</t>
+  </si>
+  <si>
+    <t>Apply 9.95 kN for 10kN load</t>
+  </si>
+  <si>
+    <t>starting axial load zeroed at 0.6092</t>
+  </si>
+  <si>
+    <t>starting horiz load zeroed at -0.3766 kN</t>
+  </si>
+  <si>
+    <t>starting axial disp zeroed at -6.7271</t>
+  </si>
+  <si>
+    <t>starting horiz disp zeroed at -24.4593 mm</t>
+  </si>
+  <si>
+    <t>experiment begins at ~1340 seconds</t>
+  </si>
+  <si>
+    <t>SPEED UP TO GET TO HIGHER FRICTION u</t>
+  </si>
+  <si>
+    <t>ended at around 5200 seconds</t>
+  </si>
+  <si>
+    <t>starting horiz load zeroed at -0.5722 kN</t>
+  </si>
+  <si>
+    <t>starting horiz disp zeroed at -24.5299 mm</t>
+  </si>
+  <si>
+    <t>starting axial disp zeroed at -5.4845</t>
+  </si>
+  <si>
+    <t>slow stick slips? Very curved</t>
+  </si>
+  <si>
+    <t>LOAD TO 20kN at 0.05kN/s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -335,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -416,6 +474,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,8 +788,8 @@
   </sheetPr>
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1941,7 +2006,7 @@
   </sheetPr>
   <dimension ref="A1:U112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -3230,7 +3295,7 @@
         <v>160</v>
       </c>
       <c r="H38" s="15">
-        <f t="shared" ref="H38:H69" si="8">G38/60</f>
+        <f t="shared" ref="H38:H54" si="8">G38/60</f>
         <v>2.6666666666666665</v>
       </c>
       <c r="I38" s="16">
@@ -4027,7 +4092,7 @@
   </sheetPr>
   <dimension ref="A1:T112"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="123" workbookViewId="0">
+    <sheetView zoomScale="64" workbookViewId="0">
       <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
@@ -5403,7 +5468,7 @@
         <v>600</v>
       </c>
       <c r="H38" s="15">
-        <f t="shared" ref="H38:H69" si="10">G38/60</f>
+        <f t="shared" ref="H38:H56" si="10">G38/60</f>
         <v>10</v>
       </c>
       <c r="I38" s="16">
@@ -6348,6 +6413,4611 @@
     </row>
     <row r="112" spans="9:9" ht="19.5" customHeight="1">
       <c r="I112" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C379C1B3-F222-4251-9631-96C885F6F532}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:T112"/>
+  <sheetViews>
+    <sheetView topLeftCell="A23" zoomScale="112" workbookViewId="0">
+      <selection activeCell="I32" sqref="B6:I32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="2" hidden="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="14.109375" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2">
+        <f>SUM(E6:E50)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="19.5" customHeight="1">
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0</v>
+      </c>
+      <c r="D6" s="30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="13">
+        <v>3</v>
+      </c>
+      <c r="F6" s="13">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" ref="G6:G10" si="0">E6/D6</f>
+        <v>600</v>
+      </c>
+      <c r="H6" s="15">
+        <f t="shared" ref="H6:H10" si="1">G6/60</f>
+        <v>10</v>
+      </c>
+      <c r="I6" s="16">
+        <f>J6</f>
+        <v>89.277777777777786</v>
+      </c>
+      <c r="J6" s="14">
+        <f>SUM(H:H)</f>
+        <v>89.277777777777786</v>
+      </c>
+      <c r="K6" s="14">
+        <f>J6/60</f>
+        <v>1.4879629629629632</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="13">
+        <f t="shared" ref="B7:B12" si="2">B6+E6</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="G7" s="13">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="H7" s="15">
+        <f t="shared" si="1"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="I7" s="16">
+        <f t="shared" ref="I7:I26" si="3">I6-H6</f>
+        <v>79.277777777777786</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="13"/>
+    </row>
+    <row r="8" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="13">
+        <f>F6+G6</f>
+        <v>600</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H8" s="15">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="I8" s="16">
+        <f t="shared" si="3"/>
+        <v>62.611111111111114</v>
+      </c>
+      <c r="L8" s="13"/>
+    </row>
+    <row r="9" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="13">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D9" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13">
+        <f>F8+G8</f>
+        <v>800</v>
+      </c>
+      <c r="G9" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H9" s="15">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I9" s="16">
+        <f t="shared" si="3"/>
+        <v>59.277777777777779</v>
+      </c>
+      <c r="L9" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="D10" s="32">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I10" s="16">
+        <f t="shared" si="3"/>
+        <v>57.611111111111114</v>
+      </c>
+      <c r="L10" s="13"/>
+    </row>
+    <row r="11" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D11" s="30">
+        <v>0.05</v>
+      </c>
+      <c r="E11" s="13">
+        <v>3</v>
+      </c>
+      <c r="F11" s="13">
+        <f>F9+G9</f>
+        <v>900</v>
+      </c>
+      <c r="G11" s="13">
+        <f>E11/D11</f>
+        <v>60</v>
+      </c>
+      <c r="H11" s="15">
+        <f>G11/60</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="16">
+        <f t="shared" si="3"/>
+        <v>56.277777777777779</v>
+      </c>
+      <c r="L11" s="13"/>
+    </row>
+    <row r="12" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="13">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="D12" s="30">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E12" s="13">
+        <v>3</v>
+      </c>
+      <c r="F12" s="13">
+        <f>F11+G11</f>
+        <v>960</v>
+      </c>
+      <c r="G12" s="13">
+        <f>E12/D12</f>
+        <v>40</v>
+      </c>
+      <c r="H12" s="15">
+        <f>G12/60</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I12" s="16">
+        <f t="shared" si="3"/>
+        <v>55.277777777777779</v>
+      </c>
+      <c r="L12" s="13"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+    </row>
+    <row r="13" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="13">
+        <f t="shared" ref="B13:B27" si="4">B12+E12</f>
+        <v>14</v>
+      </c>
+      <c r="D13" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="E13" s="13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13">
+        <f t="shared" ref="G13:G15" si="5">E13/D13</f>
+        <v>1000</v>
+      </c>
+      <c r="H13" s="15">
+        <f t="shared" ref="H13:H15" si="6">G13/60</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="I13" s="16">
+        <f t="shared" si="3"/>
+        <v>54.611111111111114</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="13">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="D14" s="30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13">
+        <f>F12+G12</f>
+        <v>1000</v>
+      </c>
+      <c r="G14" s="13">
+        <f t="shared" si="5"/>
+        <v>200</v>
+      </c>
+      <c r="H14" s="15">
+        <f t="shared" si="6"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="I14" s="16">
+        <f t="shared" si="3"/>
+        <v>37.944444444444443</v>
+      </c>
+      <c r="L14" s="13"/>
+      <c r="N14" s="17"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+    </row>
+    <row r="15" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A15" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="13">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="D15" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E15" s="13">
+        <v>1</v>
+      </c>
+      <c r="F15" s="13">
+        <f>F14+G14</f>
+        <v>1200</v>
+      </c>
+      <c r="G15" s="13">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="H15" s="15">
+        <f t="shared" si="6"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I15" s="16">
+        <f t="shared" si="3"/>
+        <v>34.611111111111107</v>
+      </c>
+      <c r="L15" s="13"/>
+    </row>
+    <row r="16" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="13">
+        <f>B15+E15</f>
+        <v>17</v>
+      </c>
+      <c r="D16" s="32">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="G16" s="2">
+        <f>E16/D16</f>
+        <v>80</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" ref="H16:H31" si="7">G16/60</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I16" s="16">
+        <f>I15-H15</f>
+        <v>32.944444444444443</v>
+      </c>
+      <c r="L16" s="13"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+    </row>
+    <row r="17" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A17" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="13">
+        <f>B16+E16</f>
+        <v>19</v>
+      </c>
+      <c r="D17" s="30">
+        <v>0.05</v>
+      </c>
+      <c r="E17" s="13">
+        <v>3</v>
+      </c>
+      <c r="F17" s="13">
+        <f>F15+G15</f>
+        <v>1300</v>
+      </c>
+      <c r="G17" s="13">
+        <f>E17/D17</f>
+        <v>60</v>
+      </c>
+      <c r="H17" s="15">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I17" s="16">
+        <f>I16-H16</f>
+        <v>31.611111111111111</v>
+      </c>
+      <c r="L17" s="13"/>
+    </row>
+    <row r="18" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A18" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="13">
+        <f>B17+E17</f>
+        <v>22</v>
+      </c>
+      <c r="D18" s="30">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E18" s="13">
+        <v>3</v>
+      </c>
+      <c r="F18" s="13">
+        <f>F17+G17</f>
+        <v>1360</v>
+      </c>
+      <c r="G18" s="13">
+        <f>E18/D18</f>
+        <v>40</v>
+      </c>
+      <c r="H18" s="15">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I18" s="16">
+        <f>I17-H17</f>
+        <v>30.611111111111111</v>
+      </c>
+      <c r="L18" s="13"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+    </row>
+    <row r="19" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="13">
+        <f>B18+E18</f>
+        <v>25</v>
+      </c>
+      <c r="D19" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E19" s="13">
+        <v>2</v>
+      </c>
+      <c r="G19" s="13">
+        <f>E19/D19</f>
+        <v>200</v>
+      </c>
+      <c r="H19" s="15">
+        <f t="shared" si="7"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="I19" s="16">
+        <f>I18-H18</f>
+        <v>29.944444444444443</v>
+      </c>
+      <c r="L19" s="13"/>
+    </row>
+    <row r="20" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="13">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0</v>
+      </c>
+      <c r="G20" s="13">
+        <v>10</v>
+      </c>
+      <c r="H20" s="15">
+        <f t="shared" si="7"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I20" s="16">
+        <f t="shared" si="3"/>
+        <v>26.611111111111111</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L20" s="13"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+    </row>
+    <row r="21" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A21" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="13">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="D21" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E21" s="13">
+        <v>1</v>
+      </c>
+      <c r="G21" s="13">
+        <f>E21/D21</f>
+        <v>100</v>
+      </c>
+      <c r="H21" s="15">
+        <f t="shared" si="7"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I21" s="16">
+        <f t="shared" si="3"/>
+        <v>26.444444444444443</v>
+      </c>
+      <c r="L21" s="13"/>
+    </row>
+    <row r="22" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="13">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="13">
+        <v>0</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0</v>
+      </c>
+      <c r="G22" s="13">
+        <v>30</v>
+      </c>
+      <c r="H22" s="15">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="I22" s="16">
+        <f t="shared" si="3"/>
+        <v>24.777777777777775</v>
+      </c>
+      <c r="L22" s="13"/>
+    </row>
+    <row r="23" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A23" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="13">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="D23" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E23" s="13">
+        <v>1</v>
+      </c>
+      <c r="G23" s="13">
+        <f>E23/D23</f>
+        <v>100</v>
+      </c>
+      <c r="H23" s="15">
+        <f t="shared" si="7"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I23" s="16">
+        <f t="shared" si="3"/>
+        <v>24.277777777777775</v>
+      </c>
+      <c r="L23" s="14"/>
+    </row>
+    <row r="24" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="13">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="13">
+        <v>0</v>
+      </c>
+      <c r="E24" s="13">
+        <v>0</v>
+      </c>
+      <c r="G24" s="13">
+        <v>300</v>
+      </c>
+      <c r="H24" s="15">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="I24" s="16">
+        <f t="shared" si="3"/>
+        <v>22.611111111111107</v>
+      </c>
+      <c r="L24" s="14"/>
+    </row>
+    <row r="25" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A25" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="13">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="D25" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E25" s="13">
+        <v>1</v>
+      </c>
+      <c r="G25" s="13">
+        <f>E25/D25</f>
+        <v>100</v>
+      </c>
+      <c r="H25" s="15">
+        <f t="shared" si="7"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I25" s="16">
+        <f t="shared" si="3"/>
+        <v>17.611111111111107</v>
+      </c>
+      <c r="L25" s="14"/>
+    </row>
+    <row r="26" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A26" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="13">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="13">
+        <v>0</v>
+      </c>
+      <c r="E26" s="13">
+        <v>0</v>
+      </c>
+      <c r="G26" s="13">
+        <v>600</v>
+      </c>
+      <c r="H26" s="15">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="I26" s="16">
+        <f t="shared" si="3"/>
+        <v>15.944444444444441</v>
+      </c>
+      <c r="L26" s="14"/>
+    </row>
+    <row r="27" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A27" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="13">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="D27" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E27" s="13">
+        <v>1</v>
+      </c>
+      <c r="G27" s="13">
+        <f>E27/D27</f>
+        <v>100</v>
+      </c>
+      <c r="H27" s="15">
+        <f t="shared" si="7"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I27" s="16">
+        <f t="shared" ref="I27" si="8">I26-H26</f>
+        <v>5.9444444444444411</v>
+      </c>
+      <c r="L27" s="14"/>
+    </row>
+    <row r="28" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A28" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="13">
+        <f>B27+E27</f>
+        <v>31</v>
+      </c>
+      <c r="D28" s="32">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2</v>
+      </c>
+      <c r="G28" s="2">
+        <f>E28/D28</f>
+        <v>80</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="7"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I28" s="16">
+        <f>I27-H27</f>
+        <v>4.2777777777777741</v>
+      </c>
+      <c r="L28" s="14"/>
+    </row>
+    <row r="29" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="13">
+        <f>B28+E28</f>
+        <v>33</v>
+      </c>
+      <c r="D29" s="30">
+        <v>0.05</v>
+      </c>
+      <c r="E29" s="13">
+        <v>3</v>
+      </c>
+      <c r="F29" s="13">
+        <f>F27+G27</f>
+        <v>100</v>
+      </c>
+      <c r="G29" s="13">
+        <f>E29/D29</f>
+        <v>60</v>
+      </c>
+      <c r="H29" s="15">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I29" s="16">
+        <f>I28-H28</f>
+        <v>2.9444444444444411</v>
+      </c>
+      <c r="L29" s="14"/>
+    </row>
+    <row r="30" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A30" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="13">
+        <f>B29+E29</f>
+        <v>36</v>
+      </c>
+      <c r="D30" s="30">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E30" s="13">
+        <v>5</v>
+      </c>
+      <c r="F30" s="13">
+        <f>F29+G29</f>
+        <v>160</v>
+      </c>
+      <c r="G30" s="13">
+        <f>E30/D30</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="H30" s="15">
+        <f t="shared" si="7"/>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="I30" s="16">
+        <f>I29-H29</f>
+        <v>1.9444444444444411</v>
+      </c>
+      <c r="L30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
+      <c r="T30" s="14"/>
+    </row>
+    <row r="31" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A31" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="13">
+        <f>B30+E30</f>
+        <v>41</v>
+      </c>
+      <c r="D31" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="E31" s="13">
+        <v>5</v>
+      </c>
+      <c r="G31" s="13">
+        <f>E31/D31</f>
+        <v>50</v>
+      </c>
+      <c r="H31" s="15">
+        <f t="shared" si="7"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I31" s="16">
+        <f>I30-H30</f>
+        <v>0.83333333333332993</v>
+      </c>
+      <c r="L31" s="14"/>
+    </row>
+    <row r="32" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B32" s="13">
+        <f>B31+E31</f>
+        <v>46</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="16"/>
+      <c r="L32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="14"/>
+    </row>
+    <row r="33" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="16"/>
+      <c r="L33" s="14"/>
+    </row>
+    <row r="34" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B34" s="13"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="16"/>
+      <c r="L34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="14"/>
+    </row>
+    <row r="35" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="16"/>
+      <c r="L35" s="14"/>
+    </row>
+    <row r="36" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B36" s="13"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="16"/>
+      <c r="L36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+    </row>
+    <row r="37" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="16"/>
+      <c r="L37" s="14"/>
+    </row>
+    <row r="38" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B38" s="13"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="16"/>
+      <c r="L38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+    </row>
+    <row r="39" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B39" s="13"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="16"/>
+      <c r="L39" s="14"/>
+    </row>
+    <row r="40" spans="2:20" ht="16.95" customHeight="1">
+      <c r="B40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="16"/>
+      <c r="L40" s="14"/>
+    </row>
+    <row r="41" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B41" s="13"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="16"/>
+      <c r="L41" s="14"/>
+    </row>
+    <row r="42" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B42" s="13"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="16"/>
+      <c r="L42" s="14"/>
+    </row>
+    <row r="43" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B43" s="13"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="16"/>
+      <c r="L43" s="14"/>
+    </row>
+    <row r="44" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="16"/>
+      <c r="L44" s="14"/>
+    </row>
+    <row r="45" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B45" s="13"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="16"/>
+      <c r="L45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="14"/>
+    </row>
+    <row r="46" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="16"/>
+      <c r="L46" s="14"/>
+    </row>
+    <row r="47" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B47" s="13"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="16"/>
+      <c r="L47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
+      <c r="T47" s="14"/>
+    </row>
+    <row r="48" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="16"/>
+      <c r="L48" s="14"/>
+    </row>
+    <row r="49" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B49" s="13"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="16"/>
+      <c r="L49" s="14"/>
+      <c r="R49" s="14"/>
+      <c r="S49" s="14"/>
+      <c r="T49" s="14"/>
+    </row>
+    <row r="50" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="16"/>
+      <c r="L50" s="14"/>
+    </row>
+    <row r="51" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B51" s="13"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="16"/>
+      <c r="L51" s="14"/>
+      <c r="R51" s="14"/>
+      <c r="S51" s="14"/>
+      <c r="T51" s="14"/>
+    </row>
+    <row r="52" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="16"/>
+      <c r="L52" s="14"/>
+    </row>
+    <row r="53" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B53" s="13"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="16"/>
+      <c r="L53" s="14"/>
+      <c r="R53" s="14"/>
+      <c r="S53" s="14"/>
+      <c r="T53" s="14"/>
+    </row>
+    <row r="54" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="16"/>
+      <c r="L54" s="14"/>
+    </row>
+    <row r="55" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B55" s="13"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="16"/>
+      <c r="L55" s="14"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="14"/>
+      <c r="T55" s="14"/>
+    </row>
+    <row r="56" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B56" s="13"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="18"/>
+      <c r="L56" s="14"/>
+    </row>
+    <row r="57" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I57" s="18"/>
+    </row>
+    <row r="58" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I58" s="18"/>
+    </row>
+    <row r="59" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I59" s="18"/>
+    </row>
+    <row r="60" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I60" s="18"/>
+    </row>
+    <row r="61" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I61" s="18"/>
+    </row>
+    <row r="62" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I62" s="18"/>
+    </row>
+    <row r="63" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I63" s="18"/>
+    </row>
+    <row r="64" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I64" s="18"/>
+    </row>
+    <row r="65" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I65" s="18"/>
+    </row>
+    <row r="66" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I66" s="18"/>
+    </row>
+    <row r="67" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I67" s="18"/>
+    </row>
+    <row r="68" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I68" s="18"/>
+    </row>
+    <row r="69" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I69" s="18"/>
+    </row>
+    <row r="70" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I70" s="18"/>
+    </row>
+    <row r="71" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I71" s="18"/>
+    </row>
+    <row r="72" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I72" s="18"/>
+    </row>
+    <row r="73" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I73" s="18"/>
+    </row>
+    <row r="74" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I74" s="18"/>
+    </row>
+    <row r="75" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I75" s="18"/>
+    </row>
+    <row r="76" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I76" s="18"/>
+    </row>
+    <row r="77" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I77" s="18"/>
+    </row>
+    <row r="78" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I78" s="18"/>
+    </row>
+    <row r="79" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I79" s="18"/>
+    </row>
+    <row r="80" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I80" s="18"/>
+    </row>
+    <row r="81" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I81" s="18"/>
+    </row>
+    <row r="82" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I82" s="18"/>
+    </row>
+    <row r="83" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I83" s="18"/>
+    </row>
+    <row r="84" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I84" s="18"/>
+    </row>
+    <row r="85" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I85" s="18"/>
+    </row>
+    <row r="86" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I86" s="18"/>
+    </row>
+    <row r="87" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I87" s="18"/>
+    </row>
+    <row r="88" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I88" s="18"/>
+    </row>
+    <row r="89" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I89" s="18"/>
+    </row>
+    <row r="90" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I90" s="18"/>
+    </row>
+    <row r="91" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I91" s="18"/>
+    </row>
+    <row r="92" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I92" s="18"/>
+    </row>
+    <row r="93" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I93" s="18"/>
+    </row>
+    <row r="94" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I94" s="18"/>
+    </row>
+    <row r="95" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I95" s="18"/>
+    </row>
+    <row r="96" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I96" s="18"/>
+    </row>
+    <row r="97" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I97" s="18"/>
+    </row>
+    <row r="98" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I98" s="18"/>
+    </row>
+    <row r="99" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I99" s="18"/>
+    </row>
+    <row r="100" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I100" s="18"/>
+    </row>
+    <row r="101" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I101" s="18"/>
+    </row>
+    <row r="102" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I102" s="18"/>
+    </row>
+    <row r="103" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I103" s="18"/>
+    </row>
+    <row r="104" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I104" s="18"/>
+    </row>
+    <row r="105" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I105" s="18"/>
+    </row>
+    <row r="106" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I106" s="18"/>
+    </row>
+    <row r="107" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I107" s="18"/>
+    </row>
+    <row r="108" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I108" s="18"/>
+    </row>
+    <row r="109" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I109" s="18"/>
+    </row>
+    <row r="110" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I110" s="18"/>
+    </row>
+    <row r="111" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I111" s="18"/>
+    </row>
+    <row r="112" spans="9:9" ht="19.5" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B4E245-299A-426E-B55C-6E0C0FEC761E}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:T112"/>
+  <sheetViews>
+    <sheetView zoomScale="113" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="2" hidden="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="14.109375" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="19.5" customHeight="1">
+      <c r="E4" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0</v>
+      </c>
+      <c r="D6" s="30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="13">
+        <v>2</v>
+      </c>
+      <c r="F6" s="13">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" ref="G6:G7" si="0">E6/D6</f>
+        <v>400</v>
+      </c>
+      <c r="H6" s="15">
+        <f t="shared" ref="H6:H7" si="1">G6/60</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="I6" s="16">
+        <f>J6</f>
+        <v>65.833333333333329</v>
+      </c>
+      <c r="J6" s="14">
+        <f>SUM(H:H)</f>
+        <v>65.833333333333329</v>
+      </c>
+      <c r="K6" s="14">
+        <f>J6/60</f>
+        <v>1.0972222222222221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="15">
+        <v>2</v>
+      </c>
+      <c r="D7" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="G7" s="13">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="H7" s="15">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I7" s="16">
+        <f t="shared" ref="I7" si="2">I6-H6</f>
+        <v>59.166666666666664</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="13"/>
+    </row>
+    <row r="8" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="15">
+        <f t="shared" ref="B8:B29" si="3">B7+E7</f>
+        <v>2.6</v>
+      </c>
+      <c r="D8" s="30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="F8" s="13">
+        <f>F6+G6</f>
+        <v>400</v>
+      </c>
+      <c r="G8" s="13">
+        <f>E8/D8</f>
+        <v>80</v>
+      </c>
+      <c r="H8" s="15">
+        <f>G8/60</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I8" s="16">
+        <f t="shared" ref="I8:I14" si="4">I7-H7</f>
+        <v>49.166666666666664</v>
+      </c>
+      <c r="L8" s="13"/>
+    </row>
+    <row r="9" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="15">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="D9" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13">
+        <f>F8+G8</f>
+        <v>480</v>
+      </c>
+      <c r="G9" s="13">
+        <f>E9/D9</f>
+        <v>100</v>
+      </c>
+      <c r="H9" s="15">
+        <f>G9/60</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I9" s="16">
+        <f t="shared" si="4"/>
+        <v>47.833333333333329</v>
+      </c>
+      <c r="L9" s="20"/>
+    </row>
+    <row r="10" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="15">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="D10" s="32">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2">
+        <f>E10/D10</f>
+        <v>80</v>
+      </c>
+      <c r="H10" s="4">
+        <f>G10/60</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I10" s="16">
+        <f t="shared" si="4"/>
+        <v>46.166666666666664</v>
+      </c>
+      <c r="L10" s="13"/>
+    </row>
+    <row r="11" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="15">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="D11" s="30">
+        <v>0.05</v>
+      </c>
+      <c r="E11" s="15">
+        <v>3</v>
+      </c>
+      <c r="F11" s="13">
+        <f>F9+G9</f>
+        <v>580</v>
+      </c>
+      <c r="G11" s="13">
+        <f>E11/D11</f>
+        <v>60</v>
+      </c>
+      <c r="H11" s="15">
+        <f>G11/60</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="16">
+        <f t="shared" si="4"/>
+        <v>44.833333333333329</v>
+      </c>
+      <c r="L11" s="13"/>
+    </row>
+    <row r="12" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="15">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="D12" s="30">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E12" s="15">
+        <v>2</v>
+      </c>
+      <c r="F12" s="13">
+        <f>F11+G11</f>
+        <v>640</v>
+      </c>
+      <c r="G12" s="13">
+        <f>E12/D12</f>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="H12" s="15">
+        <f>G12/60</f>
+        <v>0.44444444444444448</v>
+      </c>
+      <c r="I12" s="16">
+        <f t="shared" si="4"/>
+        <v>43.833333333333329</v>
+      </c>
+      <c r="L12" s="13"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+    </row>
+    <row r="13" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="15">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="D13" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="13">
+        <f t="shared" ref="G13" si="5">E13/D13</f>
+        <v>500</v>
+      </c>
+      <c r="H13" s="15">
+        <f t="shared" ref="H13" si="6">G13/60</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="I13" s="16">
+        <f t="shared" si="4"/>
+        <v>43.388888888888886</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="15">
+        <f t="shared" si="3"/>
+        <v>11.5</v>
+      </c>
+      <c r="D14" s="30">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E14" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="G14" s="13">
+        <f t="shared" ref="G14" si="7">E14/D14</f>
+        <v>46.666666666666671</v>
+      </c>
+      <c r="H14" s="15">
+        <f t="shared" ref="H14" si="8">G14/60</f>
+        <v>0.7777777777777779</v>
+      </c>
+      <c r="I14" s="16">
+        <f t="shared" si="4"/>
+        <v>35.05555555555555</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L14" s="13"/>
+      <c r="N14" s="17"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+    </row>
+    <row r="15" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A15" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="15">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="D15" s="30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E15" s="15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="13">
+        <f>F12+G12</f>
+        <v>666.66666666666663</v>
+      </c>
+      <c r="G15" s="13">
+        <f t="shared" ref="G15:G20" si="9">E15/D15</f>
+        <v>200</v>
+      </c>
+      <c r="H15" s="15">
+        <f t="shared" ref="H15:H29" si="10">G15/60</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="I15" s="16">
+        <f>I13-H13</f>
+        <v>35.05555555555555</v>
+      </c>
+      <c r="L15" s="13"/>
+    </row>
+    <row r="16" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="15">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="D16" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E16" s="15">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13">
+        <f>F15+G15</f>
+        <v>866.66666666666663</v>
+      </c>
+      <c r="G16" s="13">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="H16" s="15">
+        <f t="shared" si="10"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I16" s="16">
+        <f t="shared" ref="I16:I29" si="11">I15-H15</f>
+        <v>31.722222222222218</v>
+      </c>
+      <c r="L16" s="13"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+    </row>
+    <row r="17" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A17" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="15">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="D17" s="32">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="9"/>
+        <v>80</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="10"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I17" s="16">
+        <f t="shared" si="11"/>
+        <v>30.05555555555555</v>
+      </c>
+      <c r="L17" s="13"/>
+    </row>
+    <row r="18" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A18" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="15">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="D18" s="30">
+        <v>0.05</v>
+      </c>
+      <c r="E18" s="15">
+        <v>3</v>
+      </c>
+      <c r="F18" s="13">
+        <f>F16+G16</f>
+        <v>966.66666666666663</v>
+      </c>
+      <c r="G18" s="13">
+        <f t="shared" si="9"/>
+        <v>60</v>
+      </c>
+      <c r="H18" s="15">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="I18" s="16">
+        <f t="shared" si="11"/>
+        <v>28.722222222222218</v>
+      </c>
+      <c r="L18" s="13"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+    </row>
+    <row r="19" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="15">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="D19" s="30">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E19" s="15">
+        <v>2</v>
+      </c>
+      <c r="F19" s="13">
+        <f>F18+G18</f>
+        <v>1026.6666666666665</v>
+      </c>
+      <c r="G19" s="13">
+        <f t="shared" si="9"/>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="H19" s="15">
+        <f t="shared" si="10"/>
+        <v>0.44444444444444448</v>
+      </c>
+      <c r="I19" s="16">
+        <f t="shared" si="11"/>
+        <v>27.722222222222218</v>
+      </c>
+      <c r="L19" s="13"/>
+    </row>
+    <row r="20" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="15">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="D20" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E20" s="15">
+        <v>2</v>
+      </c>
+      <c r="G20" s="13">
+        <f t="shared" si="9"/>
+        <v>200</v>
+      </c>
+      <c r="H20" s="15">
+        <f t="shared" si="10"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="I20" s="16">
+        <f t="shared" si="11"/>
+        <v>27.277777777777775</v>
+      </c>
+      <c r="L20" s="13"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+    </row>
+    <row r="21" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A21" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="15">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0</v>
+      </c>
+      <c r="E21" s="15">
+        <v>0</v>
+      </c>
+      <c r="G21" s="13">
+        <v>10</v>
+      </c>
+      <c r="H21" s="15">
+        <f t="shared" si="10"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I21" s="16">
+        <f t="shared" si="11"/>
+        <v>23.944444444444443</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L21" s="13"/>
+    </row>
+    <row r="22" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="15">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="D22" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E22" s="15">
+        <v>1</v>
+      </c>
+      <c r="G22" s="13">
+        <f>E22/D22</f>
+        <v>100</v>
+      </c>
+      <c r="H22" s="15">
+        <f t="shared" si="10"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I22" s="16">
+        <f t="shared" si="11"/>
+        <v>23.777777777777775</v>
+      </c>
+      <c r="L22" s="13"/>
+    </row>
+    <row r="23" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A23" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="15">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0</v>
+      </c>
+      <c r="E23" s="15">
+        <v>0</v>
+      </c>
+      <c r="G23" s="13">
+        <v>30</v>
+      </c>
+      <c r="H23" s="15">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="I23" s="16">
+        <f t="shared" si="11"/>
+        <v>22.111111111111107</v>
+      </c>
+      <c r="L23" s="14"/>
+    </row>
+    <row r="24" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="15">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="D24" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E24" s="15">
+        <v>1</v>
+      </c>
+      <c r="G24" s="13">
+        <f>E24/D24</f>
+        <v>100</v>
+      </c>
+      <c r="H24" s="15">
+        <f t="shared" si="10"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I24" s="16">
+        <f t="shared" si="11"/>
+        <v>21.611111111111107</v>
+      </c>
+      <c r="L24" s="14"/>
+    </row>
+    <row r="25" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A25" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="15">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="13">
+        <v>0</v>
+      </c>
+      <c r="E25" s="15">
+        <v>0</v>
+      </c>
+      <c r="G25" s="13">
+        <v>300</v>
+      </c>
+      <c r="H25" s="15">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="I25" s="16">
+        <f t="shared" si="11"/>
+        <v>19.944444444444439</v>
+      </c>
+      <c r="L25" s="14"/>
+    </row>
+    <row r="26" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A26" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="15">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="D26" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E26" s="15">
+        <v>1</v>
+      </c>
+      <c r="G26" s="13">
+        <f>E26/D26</f>
+        <v>100</v>
+      </c>
+      <c r="H26" s="15">
+        <f t="shared" si="10"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I26" s="16">
+        <f t="shared" si="11"/>
+        <v>14.944444444444439</v>
+      </c>
+      <c r="L26" s="14"/>
+    </row>
+    <row r="27" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A27" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="15">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="13">
+        <v>0</v>
+      </c>
+      <c r="E27" s="15">
+        <v>0</v>
+      </c>
+      <c r="G27" s="13">
+        <v>600</v>
+      </c>
+      <c r="H27" s="15">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="I27" s="16">
+        <f t="shared" si="11"/>
+        <v>13.277777777777773</v>
+      </c>
+      <c r="L27" s="14"/>
+    </row>
+    <row r="28" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A28" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="15">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="D28" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E28" s="15">
+        <v>1</v>
+      </c>
+      <c r="G28" s="13">
+        <f>E28/D28</f>
+        <v>100</v>
+      </c>
+      <c r="H28" s="15">
+        <f t="shared" si="10"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I28" s="16">
+        <f t="shared" si="11"/>
+        <v>3.2777777777777732</v>
+      </c>
+      <c r="L28" s="14"/>
+    </row>
+    <row r="29" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A29" s="12"/>
+      <c r="B29" s="15">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="D29" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="E29" s="4">
+        <v>5</v>
+      </c>
+      <c r="G29" s="2">
+        <f>E29/D29</f>
+        <v>50</v>
+      </c>
+      <c r="H29" s="4">
+        <f t="shared" si="10"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I29" s="16">
+        <f t="shared" si="11"/>
+        <v>1.6111111111111065</v>
+      </c>
+      <c r="L29" s="14"/>
+    </row>
+    <row r="30" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A30" s="12"/>
+      <c r="B30" s="15">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="30"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="16"/>
+      <c r="L30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
+      <c r="T30" s="14"/>
+    </row>
+    <row r="31" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A31" s="12"/>
+      <c r="B31" s="15"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="16"/>
+      <c r="L31" s="14"/>
+    </row>
+    <row r="32" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B32" s="15"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="15"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="16"/>
+      <c r="L32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="14"/>
+    </row>
+    <row r="33" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B33" s="15"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="15"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="16"/>
+      <c r="L33" s="14"/>
+    </row>
+    <row r="34" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B34" s="13"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="16"/>
+      <c r="L34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="14"/>
+    </row>
+    <row r="35" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="16"/>
+      <c r="L35" s="14"/>
+    </row>
+    <row r="36" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B36" s="13"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="16"/>
+      <c r="L36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+    </row>
+    <row r="37" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="16"/>
+      <c r="L37" s="14"/>
+    </row>
+    <row r="38" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B38" s="13"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="16"/>
+      <c r="L38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+    </row>
+    <row r="39" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B39" s="13"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="16"/>
+      <c r="L39" s="14"/>
+    </row>
+    <row r="40" spans="2:20" ht="16.95" customHeight="1">
+      <c r="B40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="16"/>
+      <c r="L40" s="14"/>
+    </row>
+    <row r="41" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B41" s="13"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="16"/>
+      <c r="L41" s="14"/>
+    </row>
+    <row r="42" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B42" s="13"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="16"/>
+      <c r="L42" s="14"/>
+    </row>
+    <row r="43" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B43" s="13"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="16"/>
+      <c r="L43" s="14"/>
+    </row>
+    <row r="44" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="16"/>
+      <c r="L44" s="14"/>
+    </row>
+    <row r="45" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B45" s="13"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="16"/>
+      <c r="L45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="14"/>
+    </row>
+    <row r="46" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="16"/>
+      <c r="L46" s="14"/>
+    </row>
+    <row r="47" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B47" s="13"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="16"/>
+      <c r="L47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
+      <c r="T47" s="14"/>
+    </row>
+    <row r="48" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="16"/>
+      <c r="L48" s="14"/>
+    </row>
+    <row r="49" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B49" s="13"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="16"/>
+      <c r="L49" s="14"/>
+      <c r="R49" s="14"/>
+      <c r="S49" s="14"/>
+      <c r="T49" s="14"/>
+    </row>
+    <row r="50" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="16"/>
+      <c r="L50" s="14"/>
+    </row>
+    <row r="51" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B51" s="13"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="16"/>
+      <c r="L51" s="14"/>
+      <c r="R51" s="14"/>
+      <c r="S51" s="14"/>
+      <c r="T51" s="14"/>
+    </row>
+    <row r="52" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="16"/>
+      <c r="L52" s="14"/>
+    </row>
+    <row r="53" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B53" s="13"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="16"/>
+      <c r="L53" s="14"/>
+      <c r="R53" s="14"/>
+      <c r="S53" s="14"/>
+      <c r="T53" s="14"/>
+    </row>
+    <row r="54" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="16"/>
+      <c r="L54" s="14"/>
+    </row>
+    <row r="55" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B55" s="13"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="16"/>
+      <c r="L55" s="14"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="14"/>
+      <c r="T55" s="14"/>
+    </row>
+    <row r="56" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B56" s="13"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="18"/>
+      <c r="L56" s="14"/>
+    </row>
+    <row r="57" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I57" s="18"/>
+    </row>
+    <row r="58" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I58" s="18"/>
+    </row>
+    <row r="59" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I59" s="18"/>
+    </row>
+    <row r="60" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I60" s="18"/>
+    </row>
+    <row r="61" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I61" s="18"/>
+    </row>
+    <row r="62" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I62" s="18"/>
+    </row>
+    <row r="63" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I63" s="18"/>
+    </row>
+    <row r="64" spans="2:20" ht="19.5" customHeight="1">
+      <c r="I64" s="18"/>
+    </row>
+    <row r="65" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I65" s="18"/>
+    </row>
+    <row r="66" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I66" s="18"/>
+    </row>
+    <row r="67" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I67" s="18"/>
+    </row>
+    <row r="68" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I68" s="18"/>
+    </row>
+    <row r="69" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I69" s="18"/>
+    </row>
+    <row r="70" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I70" s="18"/>
+    </row>
+    <row r="71" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I71" s="18"/>
+    </row>
+    <row r="72" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I72" s="18"/>
+    </row>
+    <row r="73" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I73" s="18"/>
+    </row>
+    <row r="74" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I74" s="18"/>
+    </row>
+    <row r="75" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I75" s="18"/>
+    </row>
+    <row r="76" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I76" s="18"/>
+    </row>
+    <row r="77" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I77" s="18"/>
+    </row>
+    <row r="78" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I78" s="18"/>
+    </row>
+    <row r="79" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I79" s="18"/>
+    </row>
+    <row r="80" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I80" s="18"/>
+    </row>
+    <row r="81" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I81" s="18"/>
+    </row>
+    <row r="82" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I82" s="18"/>
+    </row>
+    <row r="83" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I83" s="18"/>
+    </row>
+    <row r="84" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I84" s="18"/>
+    </row>
+    <row r="85" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I85" s="18"/>
+    </row>
+    <row r="86" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I86" s="18"/>
+    </row>
+    <row r="87" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I87" s="18"/>
+    </row>
+    <row r="88" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I88" s="18"/>
+    </row>
+    <row r="89" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I89" s="18"/>
+    </row>
+    <row r="90" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I90" s="18"/>
+    </row>
+    <row r="91" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I91" s="18"/>
+    </row>
+    <row r="92" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I92" s="18"/>
+    </row>
+    <row r="93" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I93" s="18"/>
+    </row>
+    <row r="94" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I94" s="18"/>
+    </row>
+    <row r="95" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I95" s="18"/>
+    </row>
+    <row r="96" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I96" s="18"/>
+    </row>
+    <row r="97" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I97" s="18"/>
+    </row>
+    <row r="98" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I98" s="18"/>
+    </row>
+    <row r="99" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I99" s="18"/>
+    </row>
+    <row r="100" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I100" s="18"/>
+    </row>
+    <row r="101" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I101" s="18"/>
+    </row>
+    <row r="102" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I102" s="18"/>
+    </row>
+    <row r="103" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I103" s="18"/>
+    </row>
+    <row r="104" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I104" s="18"/>
+    </row>
+    <row r="105" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I105" s="18"/>
+    </row>
+    <row r="106" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I106" s="18"/>
+    </row>
+    <row r="107" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I107" s="18"/>
+    </row>
+    <row r="108" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I108" s="18"/>
+    </row>
+    <row r="109" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I109" s="18"/>
+    </row>
+    <row r="110" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I110" s="18"/>
+    </row>
+    <row r="111" spans="9:9" ht="19.5" customHeight="1">
+      <c r="I111" s="18"/>
+    </row>
+    <row r="112" spans="9:9" ht="19.5" customHeight="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBC5458-7016-4067-92A5-E74FF2F72316}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:T111"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="113" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="2" hidden="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="14.109375" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="19.5" customHeight="1">
+      <c r="E4" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0</v>
+      </c>
+      <c r="D6" s="30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="13">
+        <v>3</v>
+      </c>
+      <c r="F6" s="13">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" ref="G6:G10" si="0">E6/D6</f>
+        <v>600</v>
+      </c>
+      <c r="H6" s="15">
+        <f t="shared" ref="H6:H10" si="1">G6/60</f>
+        <v>10</v>
+      </c>
+      <c r="I6" s="16">
+        <f>J6</f>
+        <v>67.888888888888872</v>
+      </c>
+      <c r="J6" s="14">
+        <f>SUM(H:H)</f>
+        <v>67.888888888888872</v>
+      </c>
+      <c r="K6" s="14">
+        <f>J6/60</f>
+        <v>1.1314814814814811</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="15">
+        <f t="shared" ref="B7:B13" si="2">B6+E6</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="13">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="H7" s="15">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="I7" s="16">
+        <f t="shared" ref="I7:I12" si="3">I6-H6</f>
+        <v>57.888888888888872</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="13"/>
+    </row>
+    <row r="8" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="15">
+        <f t="shared" si="2"/>
+        <v>3.5</v>
+      </c>
+      <c r="D8" s="30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="13">
+        <f>F6+G6</f>
+        <v>600</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H8" s="15">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I8" s="16">
+        <f t="shared" si="3"/>
+        <v>49.555555555555536</v>
+      </c>
+      <c r="L8" s="13"/>
+    </row>
+    <row r="9" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="15">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D9" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13">
+        <f>F8+G8</f>
+        <v>700</v>
+      </c>
+      <c r="G9" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H9" s="15">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I9" s="16">
+        <f t="shared" si="3"/>
+        <v>47.888888888888872</v>
+      </c>
+      <c r="L9" s="20"/>
+    </row>
+    <row r="10" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="32">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I10" s="16">
+        <f t="shared" si="3"/>
+        <v>46.222222222222207</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="13"/>
+    </row>
+    <row r="11" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="15">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="30">
+        <v>0.05</v>
+      </c>
+      <c r="E11" s="15">
+        <v>3</v>
+      </c>
+      <c r="F11" s="13">
+        <f>F9+G9</f>
+        <v>800</v>
+      </c>
+      <c r="G11" s="13">
+        <f>E11/D11</f>
+        <v>60</v>
+      </c>
+      <c r="H11" s="15">
+        <f>G11/60</f>
+        <v>1</v>
+      </c>
+      <c r="I11" s="16">
+        <f t="shared" si="3"/>
+        <v>44.888888888888872</v>
+      </c>
+      <c r="L11" s="13"/>
+    </row>
+    <row r="12" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="15">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D12" s="30">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E12" s="15">
+        <v>2</v>
+      </c>
+      <c r="F12" s="13">
+        <f>F11+G11</f>
+        <v>860</v>
+      </c>
+      <c r="G12" s="13">
+        <f>E12/D12</f>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="H12" s="15">
+        <f>G12/60</f>
+        <v>0.44444444444444448</v>
+      </c>
+      <c r="I12" s="16">
+        <f t="shared" si="3"/>
+        <v>43.888888888888872</v>
+      </c>
+      <c r="L12" s="13"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+    </row>
+    <row r="13" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="15">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D13" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="13">
+        <f>F12+G12</f>
+        <v>886.66666666666663</v>
+      </c>
+      <c r="G13" s="13">
+        <f>E13/D13</f>
+        <v>500</v>
+      </c>
+      <c r="H13" s="15">
+        <f>G13/60</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="I13" s="16">
+        <f t="shared" ref="I13" si="4">I12-H12</f>
+        <v>43.444444444444429</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="15">
+        <f>B13+E13</f>
+        <v>12.5</v>
+      </c>
+      <c r="D14" s="30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="13">
+        <f t="shared" ref="G14:G16" si="5">E14/D14</f>
+        <v>100</v>
+      </c>
+      <c r="H14" s="15">
+        <f t="shared" ref="H14:H19" si="6">G14/60</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I14" s="16">
+        <f>I13-H13</f>
+        <v>35.111111111111093</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14" s="13"/>
+      <c r="N14" s="17"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+    </row>
+    <row r="15" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A15" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="15">
+        <f>B14+E14</f>
+        <v>13</v>
+      </c>
+      <c r="D15" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E15" s="15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="13">
+        <f>F12+G12</f>
+        <v>886.66666666666663</v>
+      </c>
+      <c r="G15" s="13">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="H15" s="15">
+        <f t="shared" si="6"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I15" s="16">
+        <f>I14-H14</f>
+        <v>33.444444444444429</v>
+      </c>
+      <c r="L15" s="13"/>
+    </row>
+    <row r="16" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="15">
+        <f>B15+E15</f>
+        <v>14</v>
+      </c>
+      <c r="D16" s="30">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E16" s="15">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13">
+        <f>F15+G15</f>
+        <v>986.66666666666663</v>
+      </c>
+      <c r="G16" s="13">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="H16" s="15">
+        <f t="shared" si="6"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I16" s="16">
+        <f>I15-H15</f>
+        <v>31.777777777777761</v>
+      </c>
+      <c r="L16" s="13"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+    </row>
+    <row r="17" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A17" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="15">
+        <f>B16+E16</f>
+        <v>15</v>
+      </c>
+      <c r="D17" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
+      <c r="G17" s="2">
+        <f>E17/D17</f>
+        <v>40</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="6"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I17" s="16">
+        <f t="shared" ref="I17:I23" si="7">I16-H16</f>
+        <v>31.111111111111093</v>
+      </c>
+      <c r="L17" s="13"/>
+    </row>
+    <row r="18" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A18" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="15">
+        <f>B17+E17</f>
+        <v>17</v>
+      </c>
+      <c r="D18" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="15">
+        <v>3</v>
+      </c>
+      <c r="F18" s="13">
+        <f>F16+G16</f>
+        <v>1026.6666666666665</v>
+      </c>
+      <c r="G18" s="13">
+        <f>E18/D18</f>
+        <v>30</v>
+      </c>
+      <c r="H18" s="15">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="I18" s="16">
+        <f t="shared" si="7"/>
+        <v>30.444444444444425</v>
+      </c>
+      <c r="L18" s="13"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+    </row>
+    <row r="19" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="15">
+        <v>20</v>
+      </c>
+      <c r="D19" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E19" s="15">
+        <v>2</v>
+      </c>
+      <c r="G19" s="13">
+        <f>E19/D19</f>
+        <v>200</v>
+      </c>
+      <c r="H19" s="15">
+        <f t="shared" si="6"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="I19" s="16">
+        <f t="shared" si="7"/>
+        <v>29.944444444444425</v>
+      </c>
+      <c r="L19" s="13"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+    </row>
+    <row r="20" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A20" s="12"/>
+      <c r="B20" s="15">
+        <f>B19+E19</f>
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0</v>
+      </c>
+      <c r="E20" s="15">
+        <v>0</v>
+      </c>
+      <c r="G20" s="13">
+        <v>10</v>
+      </c>
+      <c r="H20" s="15">
+        <f>G20/60</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I20" s="16">
+        <f t="shared" si="7"/>
+        <v>26.611111111111093</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L20" s="13"/>
+    </row>
+    <row r="21" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A21" s="12"/>
+      <c r="B21" s="15">
+        <f>B20+E20</f>
+        <v>22</v>
+      </c>
+      <c r="D21" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E21" s="15">
+        <v>1</v>
+      </c>
+      <c r="G21" s="13">
+        <f>E21/D21</f>
+        <v>100</v>
+      </c>
+      <c r="H21" s="15">
+        <f>G21/60</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I21" s="16">
+        <f t="shared" si="7"/>
+        <v>26.444444444444425</v>
+      </c>
+      <c r="L21" s="13"/>
+    </row>
+    <row r="22" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A22" s="12"/>
+      <c r="B22" s="15">
+        <f>B21+E21</f>
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="13">
+        <v>0</v>
+      </c>
+      <c r="E22" s="15">
+        <v>0</v>
+      </c>
+      <c r="G22" s="13">
+        <v>30</v>
+      </c>
+      <c r="H22" s="15">
+        <f>G22/60</f>
+        <v>0.5</v>
+      </c>
+      <c r="I22" s="16">
+        <f t="shared" si="7"/>
+        <v>24.777777777777757</v>
+      </c>
+      <c r="L22" s="14"/>
+    </row>
+    <row r="23" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A23" s="12"/>
+      <c r="B23" s="15">
+        <f>B22+E22</f>
+        <v>23</v>
+      </c>
+      <c r="D23" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E23" s="15">
+        <v>1</v>
+      </c>
+      <c r="G23" s="13">
+        <f>E23/D23</f>
+        <v>100</v>
+      </c>
+      <c r="H23" s="15">
+        <f>G23/60</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I23" s="16">
+        <f t="shared" si="7"/>
+        <v>24.277777777777757</v>
+      </c>
+      <c r="L23" s="14"/>
+    </row>
+    <row r="24" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A24" s="12"/>
+      <c r="B24" s="15">
+        <f>B23+E23</f>
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="13">
+        <v>0</v>
+      </c>
+      <c r="E24" s="15">
+        <v>0</v>
+      </c>
+      <c r="G24" s="13">
+        <v>300</v>
+      </c>
+      <c r="H24" s="15">
+        <f>G24/60</f>
+        <v>5</v>
+      </c>
+      <c r="I24" s="16">
+        <f>I23-H23</f>
+        <v>22.611111111111089</v>
+      </c>
+      <c r="L24" s="14"/>
+    </row>
+    <row r="25" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A25" s="12"/>
+      <c r="B25" s="15">
+        <f>B24+E24</f>
+        <v>24</v>
+      </c>
+      <c r="D25" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E25" s="15">
+        <v>1</v>
+      </c>
+      <c r="G25" s="13">
+        <f>E25/D25</f>
+        <v>100</v>
+      </c>
+      <c r="H25" s="15">
+        <f>G25/60</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I25" s="16">
+        <f>I24-H24</f>
+        <v>17.611111111111089</v>
+      </c>
+      <c r="L25" s="14"/>
+    </row>
+    <row r="26" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A26" s="12"/>
+      <c r="B26" s="15">
+        <f>B25+E25</f>
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="13">
+        <v>0</v>
+      </c>
+      <c r="E26" s="15">
+        <v>0</v>
+      </c>
+      <c r="G26" s="13">
+        <v>600</v>
+      </c>
+      <c r="H26" s="15">
+        <f>G26/60</f>
+        <v>10</v>
+      </c>
+      <c r="I26" s="16">
+        <f>I25-H25</f>
+        <v>15.944444444444423</v>
+      </c>
+      <c r="L26" s="14"/>
+    </row>
+    <row r="27" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A27" s="12"/>
+      <c r="B27" s="15">
+        <f>B26+E26</f>
+        <v>25</v>
+      </c>
+      <c r="D27" s="30">
+        <v>0.01</v>
+      </c>
+      <c r="E27" s="15">
+        <v>1</v>
+      </c>
+      <c r="G27" s="13">
+        <f>E27/D27</f>
+        <v>100</v>
+      </c>
+      <c r="H27" s="15">
+        <f>G27/60</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I27" s="16">
+        <f>I26-H26</f>
+        <v>5.9444444444444233</v>
+      </c>
+      <c r="L27" s="14"/>
+    </row>
+    <row r="28" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A28" s="12"/>
+      <c r="B28" s="15">
+        <f>B27+E27</f>
+        <v>26</v>
+      </c>
+      <c r="D28" s="32">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E28" s="4">
+        <v>2</v>
+      </c>
+      <c r="G28" s="2">
+        <f>E28/D28</f>
+        <v>80</v>
+      </c>
+      <c r="H28" s="4">
+        <f>G28/60</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I28" s="16">
+        <f>I27-H27</f>
+        <v>4.2777777777777564</v>
+      </c>
+      <c r="L28" s="14"/>
+    </row>
+    <row r="29" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A29" s="12"/>
+      <c r="B29" s="15">
+        <f>B28+E28</f>
+        <v>28</v>
+      </c>
+      <c r="D29" s="30">
+        <v>0.05</v>
+      </c>
+      <c r="E29" s="15">
+        <v>3</v>
+      </c>
+      <c r="F29" s="13">
+        <f>F27+G27</f>
+        <v>100</v>
+      </c>
+      <c r="G29" s="13">
+        <f>E29/D29</f>
+        <v>60</v>
+      </c>
+      <c r="H29" s="15">
+        <f>G29/60</f>
+        <v>1</v>
+      </c>
+      <c r="I29" s="16">
+        <f>I28-H28</f>
+        <v>2.9444444444444233</v>
+      </c>
+      <c r="L29" s="14"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="14"/>
+      <c r="T29" s="14"/>
+    </row>
+    <row r="30" spans="1:20" ht="19.5" customHeight="1">
+      <c r="A30" s="12"/>
+      <c r="B30" s="15">
+        <f>B29+E29</f>
+        <v>31</v>
+      </c>
+      <c r="D30" s="30">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E30" s="15">
+        <v>5</v>
+      </c>
+      <c r="F30" s="13">
+        <f>F29+G29</f>
+        <v>160</v>
+      </c>
+      <c r="G30" s="13">
+        <f>E30/D30</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="H30" s="15">
+        <f>G30/60</f>
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="I30" s="16">
+        <f>I29-H29</f>
+        <v>1.9444444444444233</v>
+      </c>
+      <c r="L30" s="14"/>
+    </row>
+    <row r="31" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B31" s="15">
+        <f>B30+E30</f>
+        <v>36</v>
+      </c>
+      <c r="D31" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="E31" s="15">
+        <v>5</v>
+      </c>
+      <c r="G31" s="13">
+        <f>E31/D31</f>
+        <v>50</v>
+      </c>
+      <c r="H31" s="15">
+        <f>G31/60</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I31" s="16">
+        <f>I30-H30</f>
+        <v>0.83333333333331217</v>
+      </c>
+      <c r="L31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="14"/>
+    </row>
+    <row r="32" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B32" s="15">
+        <f>B31+E31</f>
+        <v>41</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="16"/>
+      <c r="L32" s="14"/>
+    </row>
+    <row r="33" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B33" s="15"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="15"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="16"/>
+      <c r="L33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
+      <c r="T33" s="14"/>
+    </row>
+    <row r="34" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="16"/>
+      <c r="L34" s="14"/>
+    </row>
+    <row r="35" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B35" s="13"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="16"/>
+      <c r="L35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="14"/>
+    </row>
+    <row r="36" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="16"/>
+      <c r="L36" s="14"/>
+    </row>
+    <row r="37" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B37" s="13"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="16"/>
+      <c r="L37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+    </row>
+    <row r="38" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B38" s="13"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="16"/>
+      <c r="L38" s="14"/>
+    </row>
+    <row r="39" spans="2:20" ht="16.95" customHeight="1">
+      <c r="B39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="16"/>
+      <c r="L39" s="14"/>
+    </row>
+    <row r="40" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B40" s="13"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="16"/>
+      <c r="L40" s="14"/>
+    </row>
+    <row r="41" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B41" s="13"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="16"/>
+      <c r="L41" s="14"/>
+    </row>
+    <row r="42" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B42" s="13"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="16"/>
+      <c r="L42" s="14"/>
+    </row>
+    <row r="43" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="16"/>
+      <c r="L43" s="14"/>
+    </row>
+    <row r="44" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B44" s="13"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="16"/>
+      <c r="L44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
+    </row>
+    <row r="45" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="16"/>
+      <c r="L45" s="14"/>
+    </row>
+    <row r="46" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B46" s="13"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="16"/>
+      <c r="L46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
+      <c r="T46" s="14"/>
+    </row>
+    <row r="47" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="16"/>
+      <c r="L47" s="14"/>
+    </row>
+    <row r="48" spans="2:20" ht="19.5" customHeight="1">
+      <c r="B48" s="13"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="16"/>
+      <c r="L48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
+      <c r="T48" s="14"/>
+    </row>
+    <row r="49" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="16"/>
+      <c r="L49" s="14"/>
+    </row>
+    <row r="50" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B50" s="13"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="16"/>
+      <c r="L50" s="14"/>
+      <c r="R50" s="14"/>
+      <c r="S50" s="14"/>
+      <c r="T50" s="14"/>
+    </row>
+    <row r="51" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="16"/>
+      <c r="L51" s="14"/>
+    </row>
+    <row r="52" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B52" s="13"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="16"/>
+      <c r="L52" s="14"/>
+      <c r="R52" s="14"/>
+      <c r="S52" s="14"/>
+      <c r="T52" s="14"/>
+    </row>
+    <row r="53" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="16"/>
+      <c r="L53" s="14"/>
+    </row>
+    <row r="54" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B54" s="13"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="16"/>
+      <c r="L54" s="14"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="14"/>
+      <c r="T54" s="14"/>
+    </row>
+    <row r="55" spans="1:20" ht="19.5" customHeight="1">
+      <c r="B55" s="13"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="18"/>
+      <c r="L55" s="14"/>
+    </row>
+    <row r="56" spans="1:20" ht="19.5" customHeight="1">
+      <c r="I56" s="18"/>
+    </row>
+    <row r="57" spans="1:20" ht="19.5" customHeight="1">
+      <c r="I57" s="18"/>
+    </row>
+    <row r="58" spans="1:20" ht="19.5" customHeight="1">
+      <c r="I58" s="18"/>
+    </row>
+    <row r="59" spans="1:20" ht="19.5" customHeight="1">
+      <c r="I59" s="18"/>
+    </row>
+    <row r="60" spans="1:20" ht="19.5" customHeight="1">
+      <c r="I60" s="18"/>
+    </row>
+    <row r="61" spans="1:20" ht="19.5" customHeight="1">
+      <c r="I61" s="18"/>
+    </row>
+    <row r="62" spans="1:20" ht="19.5" customHeight="1">
+      <c r="I62" s="18"/>
+    </row>
+    <row r="63" spans="1:20" ht="19.5" customHeight="1">
+      <c r="I63" s="18"/>
+    </row>
+    <row r="64" spans="1:20" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A64"/>
+      <c r="B64" s="2"/>
+      <c r="C64"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="18"/>
+      <c r="M64"/>
+      <c r="N64"/>
+      <c r="O64"/>
+      <c r="P64"/>
+      <c r="Q64"/>
+    </row>
+    <row r="65" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A65"/>
+      <c r="B65" s="2"/>
+      <c r="C65"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="18"/>
+      <c r="M65"/>
+      <c r="N65"/>
+      <c r="O65"/>
+      <c r="P65"/>
+      <c r="Q65"/>
+    </row>
+    <row r="66" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A66"/>
+      <c r="B66" s="2"/>
+      <c r="C66"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="18"/>
+      <c r="M66"/>
+      <c r="N66"/>
+      <c r="O66"/>
+      <c r="P66"/>
+      <c r="Q66"/>
+    </row>
+    <row r="67" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A67"/>
+      <c r="B67" s="2"/>
+      <c r="C67"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="18"/>
+      <c r="M67"/>
+      <c r="N67"/>
+      <c r="O67"/>
+      <c r="P67"/>
+      <c r="Q67"/>
+    </row>
+    <row r="68" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A68"/>
+      <c r="B68" s="2"/>
+      <c r="C68"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="18"/>
+      <c r="M68"/>
+      <c r="N68"/>
+      <c r="O68"/>
+      <c r="P68"/>
+      <c r="Q68"/>
+    </row>
+    <row r="69" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A69"/>
+      <c r="B69" s="2"/>
+      <c r="C69"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="18"/>
+      <c r="M69"/>
+      <c r="N69"/>
+      <c r="O69"/>
+      <c r="P69"/>
+      <c r="Q69"/>
+    </row>
+    <row r="70" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A70"/>
+      <c r="B70" s="2"/>
+      <c r="C70"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="18"/>
+      <c r="M70"/>
+      <c r="N70"/>
+      <c r="O70"/>
+      <c r="P70"/>
+      <c r="Q70"/>
+    </row>
+    <row r="71" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A71"/>
+      <c r="B71" s="2"/>
+      <c r="C71"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="18"/>
+      <c r="M71"/>
+      <c r="N71"/>
+      <c r="O71"/>
+      <c r="P71"/>
+      <c r="Q71"/>
+    </row>
+    <row r="72" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A72"/>
+      <c r="B72" s="2"/>
+      <c r="C72"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="18"/>
+      <c r="M72"/>
+      <c r="N72"/>
+      <c r="O72"/>
+      <c r="P72"/>
+      <c r="Q72"/>
+    </row>
+    <row r="73" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A73"/>
+      <c r="B73" s="2"/>
+      <c r="C73"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="18"/>
+      <c r="M73"/>
+      <c r="N73"/>
+      <c r="O73"/>
+      <c r="P73"/>
+      <c r="Q73"/>
+    </row>
+    <row r="74" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A74"/>
+      <c r="B74" s="2"/>
+      <c r="C74"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="18"/>
+      <c r="M74"/>
+      <c r="N74"/>
+      <c r="O74"/>
+      <c r="P74"/>
+      <c r="Q74"/>
+    </row>
+    <row r="75" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A75"/>
+      <c r="B75" s="2"/>
+      <c r="C75"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="18"/>
+      <c r="M75"/>
+      <c r="N75"/>
+      <c r="O75"/>
+      <c r="P75"/>
+      <c r="Q75"/>
+    </row>
+    <row r="76" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A76"/>
+      <c r="B76" s="2"/>
+      <c r="C76"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="18"/>
+      <c r="M76"/>
+      <c r="N76"/>
+      <c r="O76"/>
+      <c r="P76"/>
+      <c r="Q76"/>
+    </row>
+    <row r="77" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A77"/>
+      <c r="B77" s="2"/>
+      <c r="C77"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="18"/>
+      <c r="M77"/>
+      <c r="N77"/>
+      <c r="O77"/>
+      <c r="P77"/>
+      <c r="Q77"/>
+    </row>
+    <row r="78" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A78"/>
+      <c r="B78" s="2"/>
+      <c r="C78"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="18"/>
+      <c r="M78"/>
+      <c r="N78"/>
+      <c r="O78"/>
+      <c r="P78"/>
+      <c r="Q78"/>
+    </row>
+    <row r="79" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A79"/>
+      <c r="B79" s="2"/>
+      <c r="C79"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="18"/>
+      <c r="M79"/>
+      <c r="N79"/>
+      <c r="O79"/>
+      <c r="P79"/>
+      <c r="Q79"/>
+    </row>
+    <row r="80" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A80"/>
+      <c r="B80" s="2"/>
+      <c r="C80"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="18"/>
+      <c r="M80"/>
+      <c r="N80"/>
+      <c r="O80"/>
+      <c r="P80"/>
+      <c r="Q80"/>
+    </row>
+    <row r="81" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A81"/>
+      <c r="B81" s="2"/>
+      <c r="C81"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="18"/>
+      <c r="M81"/>
+      <c r="N81"/>
+      <c r="O81"/>
+      <c r="P81"/>
+      <c r="Q81"/>
+    </row>
+    <row r="82" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A82"/>
+      <c r="B82" s="2"/>
+      <c r="C82"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="18"/>
+      <c r="M82"/>
+      <c r="N82"/>
+      <c r="O82"/>
+      <c r="P82"/>
+      <c r="Q82"/>
+    </row>
+    <row r="83" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A83"/>
+      <c r="B83" s="2"/>
+      <c r="C83"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="18"/>
+      <c r="M83"/>
+      <c r="N83"/>
+      <c r="O83"/>
+      <c r="P83"/>
+      <c r="Q83"/>
+    </row>
+    <row r="84" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A84"/>
+      <c r="B84" s="2"/>
+      <c r="C84"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="18"/>
+      <c r="M84"/>
+      <c r="N84"/>
+      <c r="O84"/>
+      <c r="P84"/>
+      <c r="Q84"/>
+    </row>
+    <row r="85" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A85"/>
+      <c r="B85" s="2"/>
+      <c r="C85"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="18"/>
+      <c r="M85"/>
+      <c r="N85"/>
+      <c r="O85"/>
+      <c r="P85"/>
+      <c r="Q85"/>
+    </row>
+    <row r="86" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A86"/>
+      <c r="B86" s="2"/>
+      <c r="C86"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="18"/>
+      <c r="M86"/>
+      <c r="N86"/>
+      <c r="O86"/>
+      <c r="P86"/>
+      <c r="Q86"/>
+    </row>
+    <row r="87" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A87"/>
+      <c r="B87" s="2"/>
+      <c r="C87"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="18"/>
+      <c r="M87"/>
+      <c r="N87"/>
+      <c r="O87"/>
+      <c r="P87"/>
+      <c r="Q87"/>
+    </row>
+    <row r="88" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A88"/>
+      <c r="B88" s="2"/>
+      <c r="C88"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="18"/>
+      <c r="M88"/>
+      <c r="N88"/>
+      <c r="O88"/>
+      <c r="P88"/>
+      <c r="Q88"/>
+    </row>
+    <row r="89" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A89"/>
+      <c r="B89" s="2"/>
+      <c r="C89"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="18"/>
+      <c r="M89"/>
+      <c r="N89"/>
+      <c r="O89"/>
+      <c r="P89"/>
+      <c r="Q89"/>
+    </row>
+    <row r="90" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A90"/>
+      <c r="B90" s="2"/>
+      <c r="C90"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="18"/>
+      <c r="M90"/>
+      <c r="N90"/>
+      <c r="O90"/>
+      <c r="P90"/>
+      <c r="Q90"/>
+    </row>
+    <row r="91" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A91"/>
+      <c r="B91" s="2"/>
+      <c r="C91"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="18"/>
+      <c r="M91"/>
+      <c r="N91"/>
+      <c r="O91"/>
+      <c r="P91"/>
+      <c r="Q91"/>
+    </row>
+    <row r="92" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A92"/>
+      <c r="B92" s="2"/>
+      <c r="C92"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="18"/>
+      <c r="M92"/>
+      <c r="N92"/>
+      <c r="O92"/>
+      <c r="P92"/>
+      <c r="Q92"/>
+    </row>
+    <row r="93" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A93"/>
+      <c r="B93" s="2"/>
+      <c r="C93"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="18"/>
+      <c r="M93"/>
+      <c r="N93"/>
+      <c r="O93"/>
+      <c r="P93"/>
+      <c r="Q93"/>
+    </row>
+    <row r="94" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A94"/>
+      <c r="B94" s="2"/>
+      <c r="C94"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="18"/>
+      <c r="M94"/>
+      <c r="N94"/>
+      <c r="O94"/>
+      <c r="P94"/>
+      <c r="Q94"/>
+    </row>
+    <row r="95" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A95"/>
+      <c r="B95" s="2"/>
+      <c r="C95"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="18"/>
+      <c r="M95"/>
+      <c r="N95"/>
+      <c r="O95"/>
+      <c r="P95"/>
+      <c r="Q95"/>
+    </row>
+    <row r="96" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A96"/>
+      <c r="B96" s="2"/>
+      <c r="C96"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="18"/>
+      <c r="M96"/>
+      <c r="N96"/>
+      <c r="O96"/>
+      <c r="P96"/>
+      <c r="Q96"/>
+    </row>
+    <row r="97" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A97"/>
+      <c r="B97" s="2"/>
+      <c r="C97"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="18"/>
+      <c r="M97"/>
+      <c r="N97"/>
+      <c r="O97"/>
+      <c r="P97"/>
+      <c r="Q97"/>
+    </row>
+    <row r="98" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A98"/>
+      <c r="B98" s="2"/>
+      <c r="C98"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="18"/>
+      <c r="M98"/>
+      <c r="N98"/>
+      <c r="O98"/>
+      <c r="P98"/>
+      <c r="Q98"/>
+    </row>
+    <row r="99" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A99"/>
+      <c r="B99" s="2"/>
+      <c r="C99"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="18"/>
+      <c r="M99"/>
+      <c r="N99"/>
+      <c r="O99"/>
+      <c r="P99"/>
+      <c r="Q99"/>
+    </row>
+    <row r="100" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A100"/>
+      <c r="B100" s="2"/>
+      <c r="C100"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="18"/>
+      <c r="M100"/>
+      <c r="N100"/>
+      <c r="O100"/>
+      <c r="P100"/>
+      <c r="Q100"/>
+    </row>
+    <row r="101" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A101"/>
+      <c r="B101" s="2"/>
+      <c r="C101"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="18"/>
+      <c r="M101"/>
+      <c r="N101"/>
+      <c r="O101"/>
+      <c r="P101"/>
+      <c r="Q101"/>
+    </row>
+    <row r="102" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A102"/>
+      <c r="B102" s="2"/>
+      <c r="C102"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="18"/>
+      <c r="M102"/>
+      <c r="N102"/>
+      <c r="O102"/>
+      <c r="P102"/>
+      <c r="Q102"/>
+    </row>
+    <row r="103" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A103"/>
+      <c r="B103" s="2"/>
+      <c r="C103"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="4"/>
+      <c r="I103" s="18"/>
+      <c r="M103"/>
+      <c r="N103"/>
+      <c r="O103"/>
+      <c r="P103"/>
+      <c r="Q103"/>
+    </row>
+    <row r="104" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A104"/>
+      <c r="B104" s="2"/>
+      <c r="C104"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="4"/>
+      <c r="I104" s="18"/>
+      <c r="M104"/>
+      <c r="N104"/>
+      <c r="O104"/>
+      <c r="P104"/>
+      <c r="Q104"/>
+    </row>
+    <row r="105" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A105"/>
+      <c r="B105" s="2"/>
+      <c r="C105"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="4"/>
+      <c r="I105" s="18"/>
+      <c r="M105"/>
+      <c r="N105"/>
+      <c r="O105"/>
+      <c r="P105"/>
+      <c r="Q105"/>
+    </row>
+    <row r="106" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A106"/>
+      <c r="B106" s="2"/>
+      <c r="C106"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="18"/>
+      <c r="M106"/>
+      <c r="N106"/>
+      <c r="O106"/>
+      <c r="P106"/>
+      <c r="Q106"/>
+    </row>
+    <row r="107" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A107"/>
+      <c r="B107" s="2"/>
+      <c r="C107"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="18"/>
+      <c r="M107"/>
+      <c r="N107"/>
+      <c r="O107"/>
+      <c r="P107"/>
+      <c r="Q107"/>
+    </row>
+    <row r="108" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A108"/>
+      <c r="B108" s="2"/>
+      <c r="C108"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="18"/>
+      <c r="M108"/>
+      <c r="N108"/>
+      <c r="O108"/>
+      <c r="P108"/>
+      <c r="Q108"/>
+    </row>
+    <row r="109" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A109"/>
+      <c r="B109" s="2"/>
+      <c r="C109"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="18"/>
+      <c r="M109"/>
+      <c r="N109"/>
+      <c r="O109"/>
+      <c r="P109"/>
+      <c r="Q109"/>
+    </row>
+    <row r="110" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A110"/>
+      <c r="B110" s="2"/>
+      <c r="C110"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="4"/>
+      <c r="I110" s="18"/>
+      <c r="M110"/>
+      <c r="N110"/>
+      <c r="O110"/>
+      <c r="P110"/>
+      <c r="Q110"/>
+    </row>
+    <row r="111" spans="1:17" s="3" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A111"/>
+      <c r="B111" s="2"/>
+      <c r="C111"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="5"/>
+      <c r="M111"/>
+      <c r="N111"/>
+      <c r="O111"/>
+      <c r="P111"/>
+      <c r="Q111"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>